<commit_message>
Session Handel test update
</commit_message>
<xml_diff>
--- a/DB_Structure.xlsx
+++ b/DB_Structure.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -465,20 +466,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -502,6 +491,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -785,36 +786,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:C38"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="30" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="30" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="26" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="26" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="37"/>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
@@ -907,16 +908,16 @@
       <c r="B13" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="34" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22" t="s">
+      <c r="A14" s="20"/>
+      <c r="B14" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="23"/>
+      <c r="C14" s="35"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
@@ -952,7 +953,7 @@
       <c r="B18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="36" t="s">
         <v>31</v>
       </c>
     </row>
@@ -961,7 +962,7 @@
       <c r="B19" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="25"/>
+      <c r="C19" s="37"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
@@ -970,48 +971,48 @@
       <c r="B20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="24" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="24" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="28"/>
+      <c r="C23" s="24"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="28"/>
+      <c r="C24" s="24"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
-      <c r="B25" s="22" t="s">
+      <c r="A25" s="20"/>
+      <c r="B25" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="25" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1065,66 +1066,66 @@
       <c r="B31" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="28"/>
+      <c r="C32" s="24"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="24" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="24" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="28"/>
+      <c r="C35" s="24"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="24" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="27"/>
+      <c r="A37" s="23"/>
       <c r="B37" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="24" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="21"/>
-      <c r="B38" s="22" t="s">
+      <c r="A38" s="20"/>
+      <c r="B38" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="29"/>
+      <c r="C38" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>